<commit_message>
updated file list to include overall concentration of cells per ml
</commit_message>
<xml_diff>
--- a/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Filename</t>
   </si>
@@ -47,7 +47,52 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>beads</t>
+    <t>D20151029T193910</t>
+  </si>
+  <si>
+    <t>D20151029T202442</t>
+  </si>
+  <si>
+    <t>D20151029T203651</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>D20151029T210223</t>
+  </si>
+  <si>
+    <t>D20151029T214652</t>
+  </si>
+  <si>
+    <t>D20151029T215618</t>
+  </si>
+  <si>
+    <t>D20151029T220128</t>
+  </si>
+  <si>
+    <t>D20151029T220740</t>
+  </si>
+  <si>
+    <t>D20151029T221754</t>
+  </si>
+  <si>
+    <t>D20151029T223228</t>
+  </si>
+  <si>
+    <t>D20151029T225342</t>
+  </si>
+  <si>
+    <t>D20151029T231617</t>
+  </si>
+  <si>
+    <t>D20151029T232145</t>
+  </si>
+  <si>
+    <t>beads in FSW</t>
+  </si>
+  <si>
+    <t>D20151029T213311</t>
   </si>
 </sst>
 </file>
@@ -83,8 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,17 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -388,7 +437,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -397,19 +446,261 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5464.0161750868401</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5896.1852217658998</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6144.90150733874</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6640.3057811756598</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6718.5436046208097</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6824.3387591719502</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5822.4906469859698</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6538.2808861286203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7507.2133133217303</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7859.08168935498</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7680.6059020955799</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8103.3769298114703</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8049.1286860790296</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7782.2739125382104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8426.7018632295403</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new round of exp vert vs horz, first need vert runs to even out and run consistently
</commit_message>
<xml_diff>
--- a/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\IFCB_vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\IFCB_vehicles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="5085" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VvsHdiffVol_nogood" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Filename</t>
   </si>
@@ -93,6 +94,36 @@
   </si>
   <si>
     <t>D20151029T213311</t>
+  </si>
+  <si>
+    <t>9um beads</t>
+  </si>
+  <si>
+    <t>2nd exp first file after high conc runs of last exp</t>
+  </si>
+  <si>
+    <t>Comments2</t>
+  </si>
+  <si>
+    <t>D20151103T150629</t>
+  </si>
+  <si>
+    <t>D20151103T145610</t>
+  </si>
+  <si>
+    <t>D20151103T151633</t>
+  </si>
+  <si>
+    <t>D20151103T152713</t>
+  </si>
+  <si>
+    <t>realize incorrectly running 2ml when want to run 5ml</t>
+  </si>
+  <si>
+    <t>D20151103T154933</t>
+  </si>
+  <si>
+    <t>2?</t>
   </si>
 </sst>
 </file>
@@ -415,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,4 +734,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>621</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>585</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>583</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>633</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated files from today, done with vertical, going to horz 5ml repeated
</commit_message>
<xml_diff>
--- a/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>Filename</t>
   </si>
@@ -124,6 +124,39 @@
   </si>
   <si>
     <t>2?</t>
+  </si>
+  <si>
+    <t>D20151103T161152</t>
+  </si>
+  <si>
+    <t>D20151103T163411</t>
+  </si>
+  <si>
+    <t>use all signals</t>
+  </si>
+  <si>
+    <t>ml_analyzed</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>inhibittime</t>
+  </si>
+  <si>
+    <t>numtriggers</t>
+  </si>
+  <si>
+    <t>D20151103T165631</t>
+  </si>
+  <si>
+    <t>&lt;5</t>
+  </si>
+  <si>
+    <t>sampled ended early because concentration consistent enough to move on to next stage: horz 5ml runs</t>
+  </si>
+  <si>
+    <t>9um beads, use all signals</t>
   </si>
 </sst>
 </file>
@@ -738,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,11 +783,13 @@
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,14 +802,26 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -787,14 +834,17 @@
       <c r="D2">
         <v>621</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -807,11 +857,14 @@
       <c r="D3">
         <v>585</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -824,14 +877,17 @@
       <c r="D4">
         <v>583</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -844,11 +900,14 @@
       <c r="D5">
         <v>633</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -858,8 +917,130 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6">
+        <v>637.70000000000005</v>
+      </c>
+      <c r="E6">
+        <v>4.0865</v>
+      </c>
+      <c r="F6">
+        <v>1198.04</v>
+      </c>
+      <c r="G6">
+        <v>202.27199999999999</v>
+      </c>
+      <c r="H6">
+        <v>2606</v>
+      </c>
+      <c r="I6" t="s">
         <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>636.6</v>
+      </c>
+      <c r="E7">
+        <v>4.0888</v>
+      </c>
+      <c r="F7">
+        <v>1198</v>
+      </c>
+      <c r="G7">
+        <v>204.11</v>
+      </c>
+      <c r="H7">
+        <v>2603</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>635.6</v>
+      </c>
+      <c r="E8">
+        <v>4.0873999999999997</v>
+      </c>
+      <c r="F8">
+        <v>1198</v>
+      </c>
+      <c r="G8">
+        <v>201.6</v>
+      </c>
+      <c r="H8">
+        <v>2598</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>600</v>
+      </c>
+      <c r="E9">
+        <v>1.1843999999999999</v>
+      </c>
+      <c r="F9">
+        <v>351.2</v>
+      </c>
+      <c r="G9">
+        <v>56.13</v>
+      </c>
+      <c r="H9">
+        <v>711</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further updated filenames with concentrations. moving into horizontal runs
</commit_message>
<xml_diff>
--- a/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
+++ b/IFCB_vehicles/VehicleLabExperimentFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="54">
   <si>
     <t>Filename</t>
   </si>
@@ -123,9 +123,6 @@
     <t>D20151103T154933</t>
   </si>
   <si>
-    <t>2?</t>
-  </si>
-  <si>
     <t>D20151103T161152</t>
   </si>
   <si>
@@ -150,13 +147,46 @@
     <t>D20151103T165631</t>
   </si>
   <si>
-    <t>&lt;5</t>
-  </si>
-  <si>
     <t>sampled ended early because concentration consistent enough to move on to next stage: horz 5ml runs</t>
   </si>
   <si>
     <t>9um beads, use all signals</t>
+  </si>
+  <si>
+    <t>D20151103T170912</t>
+  </si>
+  <si>
+    <t>D20151103T173215</t>
+  </si>
+  <si>
+    <t>D20151103T175435</t>
+  </si>
+  <si>
+    <t>First horz sample</t>
+  </si>
+  <si>
+    <t>ypos moved up a bit (matlab) makes laser off more in PMTB signals</t>
+  </si>
+  <si>
+    <t>D20151103T181654</t>
+  </si>
+  <si>
+    <t>5*</t>
+  </si>
+  <si>
+    <t>2*</t>
+  </si>
+  <si>
+    <t>D20151103T183914</t>
+  </si>
+  <si>
+    <t>D20151103T190133</t>
+  </si>
+  <si>
+    <t>D20151103T192802</t>
+  </si>
+  <si>
+    <t>first run switched to 4ml from 5ml</t>
   </si>
 </sst>
 </file>
@@ -771,10 +801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,16 +833,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -825,8 +855,8 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -834,6 +864,18 @@
       <c r="D2">
         <v>621</v>
       </c>
+      <c r="E2">
+        <v>1.6185</v>
+      </c>
+      <c r="F2">
+        <v>478</v>
+      </c>
+      <c r="G2">
+        <v>73.459999999999994</v>
+      </c>
+      <c r="H2">
+        <v>1005</v>
+      </c>
       <c r="I2" t="s">
         <v>23</v>
       </c>
@@ -841,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -857,11 +899,23 @@
       <c r="D3">
         <v>585</v>
       </c>
+      <c r="E3">
+        <v>1.637</v>
+      </c>
+      <c r="F3">
+        <v>478</v>
+      </c>
+      <c r="G3">
+        <v>69.22</v>
+      </c>
+      <c r="H3">
+        <v>957</v>
+      </c>
       <c r="I3" t="s">
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -869,7 +923,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -877,6 +931,18 @@
       <c r="D4">
         <v>583</v>
       </c>
+      <c r="E4">
+        <v>1.6419999999999999</v>
+      </c>
+      <c r="F4">
+        <v>478</v>
+      </c>
+      <c r="G4">
+        <v>68.44</v>
+      </c>
+      <c r="H4">
+        <v>958</v>
+      </c>
       <c r="I4" t="s">
         <v>23</v>
       </c>
@@ -884,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -900,11 +966,23 @@
       <c r="D5">
         <v>633</v>
       </c>
+      <c r="E5">
+        <v>4.1097999999999999</v>
+      </c>
+      <c r="F5">
+        <v>1198</v>
+      </c>
+      <c r="G5">
+        <v>211.6</v>
+      </c>
+      <c r="H5">
+        <v>2605</v>
+      </c>
       <c r="I5" t="s">
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -936,12 +1014,12 @@
         <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -968,12 +1046,12 @@
         <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -1000,15 +1078,15 @@
         <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1029,18 +1107,207 @@
         <v>711</v>
       </c>
       <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="J9" t="s">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>580</v>
+      </c>
+      <c r="E10">
+        <v>4.1439000000000004</v>
+      </c>
+      <c r="F10">
+        <v>1198</v>
+      </c>
+      <c r="G10">
+        <v>187</v>
+      </c>
+      <c r="H10">
+        <v>2403</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>580.1</v>
+      </c>
+      <c r="E11">
+        <v>4.1440999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1198</v>
+      </c>
+      <c r="G11">
+        <v>188.78</v>
+      </c>
+      <c r="H11">
+        <v>2404</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>591.6</v>
+      </c>
+      <c r="E12">
+        <v>4.1295999999999999</v>
+      </c>
+      <c r="F12">
+        <v>1198</v>
+      </c>
+      <c r="G12">
+        <v>190.1</v>
+      </c>
+      <c r="H12">
+        <v>2443</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>565.70000000000005</v>
+      </c>
+      <c r="E13">
+        <v>4.1664000000000003</v>
+      </c>
+      <c r="F13">
+        <v>1198</v>
+      </c>
+      <c r="G13">
+        <v>183.6</v>
+      </c>
+      <c r="H13">
+        <v>2357</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>543.4</v>
+      </c>
+      <c r="E14">
+        <v>4.2340999999999998</v>
+      </c>
+      <c r="F14">
+        <v>1198</v>
+      </c>
+      <c r="G14">
+        <v>181.79</v>
+      </c>
+      <c r="H14">
+        <v>2301</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>578.29999999999995</v>
+      </c>
+      <c r="E15">
+        <v>4.1193</v>
+      </c>
+      <c r="F15">
+        <v>1198</v>
+      </c>
+      <c r="G15">
+        <v>192.3</v>
+      </c>
+      <c r="H15">
+        <v>2382</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>